<commit_message>
Bearbeitung StoryCards.xlsx nach falsch eingabe
</commit_message>
<xml_diff>
--- a/StoryCards.xlsx
+++ b/StoryCards.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="375" windowWidth="13875" windowHeight="5160"/>
@@ -12,14 +12,14 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$7:$M$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$7:$M$34</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="68">
   <si>
     <t>ID</t>
   </si>
@@ -190,15 +190,6 @@
   </si>
   <si>
     <t>Implementierung des Algorithmus</t>
-  </si>
-  <si>
-    <t>Überarbeitung GUI</t>
-  </si>
-  <si>
-    <t>Überarbeitung der GUI mit MIcrosoftBlend</t>
-  </si>
-  <si>
-    <t>12h</t>
   </si>
   <si>
     <t>Schlufter, Thomas</t>
@@ -237,8 +228,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -310,7 +301,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -324,7 +315,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -339,7 +330,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -413,6 +404,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -447,6 +439,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -622,14 +615,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -645,7 +638,7 @@
     <col min="13" max="13" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="33.75">
+    <row r="1" spans="1:14" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
         <v>18</v>
       </c>
@@ -654,7 +647,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -676,7 +669,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
@@ -692,7 +685,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -708,7 +701,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
@@ -721,7 +714,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="25.5">
+    <row r="7" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -763,7 +756,7 @@
       </c>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -804,7 +797,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -845,7 +838,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -886,7 +879,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -927,7 +920,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
@@ -962,7 +955,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
@@ -997,7 +990,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7</v>
       </c>
@@ -1029,7 +1022,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>8</v>
       </c>
@@ -1058,27 +1051,24 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="E16" s="3">
         <v>40822</v>
       </c>
       <c r="F16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G16" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="H16" t="s">
         <v>45</v>
@@ -1086,11 +1076,8 @@
       <c r="I16" t="s">
         <v>58</v>
       </c>
-      <c r="K16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10</v>
       </c>
@@ -1098,7 +1085,7 @@
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E17" s="3">
         <v>40822</v>
@@ -1107,83 +1094,89 @@
         <v>16</v>
       </c>
       <c r="G17" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" t="s">
         <v>60</v>
       </c>
-      <c r="H17" t="s">
-        <v>45</v>
-      </c>
-      <c r="I17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="D18" t="s">
+        <v>34</v>
       </c>
       <c r="E18" s="3">
-        <v>40822</v>
+        <v>40795</v>
       </c>
       <c r="F18" t="s">
         <v>16</v>
       </c>
       <c r="G18" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="H18" t="s">
+        <v>45</v>
+      </c>
+      <c r="I18" t="s">
         <v>62</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
+        <v>31</v>
+      </c>
+      <c r="K18" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="L18" t="s">
+        <v>63</v>
+      </c>
+      <c r="M18" s="3">
+        <v>40795</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
         <v>34</v>
       </c>
       <c r="E19" s="3">
-        <v>40795</v>
+        <v>40822</v>
       </c>
       <c r="F19" t="s">
         <v>16</v>
       </c>
       <c r="G19" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="H19" t="s">
         <v>45</v>
       </c>
       <c r="I19" t="s">
+        <v>64</v>
+      </c>
+      <c r="K19" t="s">
         <v>65</v>
       </c>
-      <c r="J19" t="s">
-        <v>31</v>
-      </c>
-      <c r="K19" t="s">
-        <v>66</v>
-      </c>
-      <c r="L19" t="s">
-        <v>66</v>
-      </c>
-      <c r="M19" s="3">
-        <v>40795</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>13</v>
       </c>
@@ -1191,10 +1184,10 @@
         <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="E20" s="3">
         <v>40822</v>
@@ -1202,47 +1195,15 @@
       <c r="F20" t="s">
         <v>16</v>
       </c>
-      <c r="G20" t="s">
-        <v>16</v>
-      </c>
       <c r="H20" t="s">
         <v>45</v>
       </c>
       <c r="I20" t="s">
         <v>67</v>
       </c>
-      <c r="K20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21">
-        <v>14</v>
-      </c>
-      <c r="B21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" s="3">
-        <v>40822</v>
-      </c>
-      <c r="F21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" t="s">
-        <v>45</v>
-      </c>
-      <c r="I21" t="s">
-        <v>70</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A7:M35"/>
+  <autoFilter ref="A7:M34"/>
   <mergeCells count="5">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A1:E1"/>
@@ -1259,31 +1220,31 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8:B35">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="fertig">
-      <formula>NOT(ISERROR(SEARCH("fertig",B8)))</formula>
+  <conditionalFormatting sqref="B8:B34">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="jungfräulich">
+      <formula>NOT(ISERROR(SEARCH("jungfräulich",B8)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="in Arbeit">
       <formula>NOT(ISERROR(SEARCH("in Arbeit",B8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="jungfräulich">
-      <formula>NOT(ISERROR(SEARCH("jungfräulich",B8)))</formula>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="fertig">
+      <formula>NOT(ISERROR(SEARCH("fertig",B8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F8:F35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F8:F34">
       <formula1>$D$2:$H$2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C34">
       <formula1>$D$3:$F$3</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B8:B35">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B8:B34">
       <formula1>$D$4:$F$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J8:J35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J8:J34">
       <formula1>$D$5:$E$5</formula1>
     </dataValidation>
-    <dataValidation showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="G8:G35"/>
+    <dataValidation showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="G8:G34"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -1291,24 +1252,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
-ticjet zu neuen anforderungen fertig
</commit_message>
<xml_diff>
--- a/StoryCards.xlsx
+++ b/StoryCards.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="375" windowWidth="13875" windowHeight="5160"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="68">
   <si>
     <t>ID</t>
   </si>
@@ -228,8 +228,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -330,7 +330,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -404,7 +404,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -439,7 +438,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -615,14 +613,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -638,7 +636,7 @@
     <col min="13" max="13" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="33.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:14" ht="33.75">
       <c r="A1" s="5" t="s">
         <v>18</v>
       </c>
@@ -647,7 +645,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -669,7 +667,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
@@ -685,7 +683,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -701,7 +699,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
@@ -714,7 +712,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="25.5">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -756,7 +754,7 @@
       </c>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="A8">
         <v>1</v>
       </c>
@@ -797,7 +795,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="A9">
         <v>2</v>
       </c>
@@ -838,7 +836,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="A10">
         <v>3</v>
       </c>
@@ -879,7 +877,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11">
         <v>4</v>
       </c>
@@ -920,7 +918,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="A12">
         <v>5</v>
       </c>
@@ -955,7 +953,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14">
       <c r="A13">
         <v>6</v>
       </c>
@@ -990,7 +988,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14">
       <c r="A14">
         <v>7</v>
       </c>
@@ -1022,7 +1020,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14">
       <c r="A15">
         <v>8</v>
       </c>
@@ -1051,7 +1049,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14">
       <c r="A16">
         <v>9</v>
       </c>
@@ -1077,7 +1075,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13">
       <c r="A17">
         <v>10</v>
       </c>
@@ -1103,7 +1101,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13">
       <c r="A18">
         <v>11</v>
       </c>
@@ -1144,12 +1142,12 @@
         <v>40795</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13">
       <c r="A19">
         <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
         <v>25</v>
@@ -1172,11 +1170,20 @@
       <c r="I19" t="s">
         <v>64</v>
       </c>
+      <c r="J19" t="s">
+        <v>31</v>
+      </c>
       <c r="K19" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>63</v>
+      </c>
+      <c r="M19" s="3">
+        <v>40822</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20">
         <v>13</v>
       </c>
@@ -1252,24 +1259,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
-nach Planung in der Veranstaltung
</commit_message>
<xml_diff>
--- a/StoryCards.xlsx
+++ b/StoryCards.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="73">
   <si>
     <t>ID</t>
   </si>
@@ -192,9 +192,6 @@
     <t>Implementierung des Algorithmus</t>
   </si>
   <si>
-    <t>Schlufter, Thomas</t>
-  </si>
-  <si>
     <t>Volle Funktionalität des Programms</t>
   </si>
   <si>
@@ -222,7 +219,25 @@
     <t>Datenausgabe</t>
   </si>
   <si>
-    <t>Ergebnis speichern</t>
+    <t>Thomas, Mrosk/Schlufter</t>
+  </si>
+  <si>
+    <t>Ergebnis speichern(xml oder txt)</t>
+  </si>
+  <si>
+    <t>Ablaufplan und Formeln erstellen</t>
+  </si>
+  <si>
+    <t>Ablaufplan studieren</t>
+  </si>
+  <si>
+    <t>Endabnahme</t>
+  </si>
+  <si>
+    <t>alle</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -617,7 +632,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -943,6 +958,12 @@
       <c r="H12" t="s">
         <v>43</v>
       </c>
+      <c r="I12" t="s">
+        <v>69</v>
+      </c>
+      <c r="J12" t="s">
+        <v>31</v>
+      </c>
       <c r="K12" t="s">
         <v>52</v>
       </c>
@@ -978,6 +999,12 @@
       <c r="H13" t="s">
         <v>44</v>
       </c>
+      <c r="I13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J13" t="s">
+        <v>31</v>
+      </c>
       <c r="K13" t="s">
         <v>52</v>
       </c>
@@ -1054,11 +1081,14 @@
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
         <v>24</v>
       </c>
+      <c r="D16" t="s">
+        <v>70</v>
+      </c>
       <c r="E16" s="3">
         <v>40822</v>
       </c>
@@ -1066,13 +1096,22 @@
         <v>16</v>
       </c>
       <c r="G16" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="H16" t="s">
         <v>45</v>
       </c>
       <c r="I16" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="K16" t="s">
+        <v>72</v>
+      </c>
+      <c r="L16" t="s">
+        <v>72</v>
+      </c>
+      <c r="M16" s="3">
+        <v>40847</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -1080,11 +1119,14 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
         <v>25</v>
       </c>
+      <c r="D17" t="s">
+        <v>55</v>
+      </c>
       <c r="E17" s="3">
         <v>40822</v>
       </c>
@@ -1095,10 +1137,10 @@
         <v>51</v>
       </c>
       <c r="H17" t="s">
+        <v>58</v>
+      </c>
+      <c r="I17" t="s">
         <v>59</v>
-      </c>
-      <c r="I17" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -1121,22 +1163,22 @@
         <v>16</v>
       </c>
       <c r="G18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H18" t="s">
         <v>45</v>
       </c>
       <c r="I18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J18" t="s">
         <v>31</v>
       </c>
       <c r="K18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M18" s="3">
         <v>40795</v>
@@ -1168,16 +1210,16 @@
         <v>45</v>
       </c>
       <c r="I19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J19" t="s">
         <v>31</v>
       </c>
       <c r="K19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M19" s="3">
         <v>40822</v>
@@ -1194,7 +1236,7 @@
         <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E20" s="3">
         <v>40822</v>
@@ -1202,11 +1244,17 @@
       <c r="F20" t="s">
         <v>16</v>
       </c>
+      <c r="G20" t="s">
+        <v>66</v>
+      </c>
       <c r="H20" t="s">
         <v>45</v>
       </c>
       <c r="I20" t="s">
         <v>67</v>
+      </c>
+      <c r="K20" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Erstellen von neuen Einträgen in StoryCards.xlsx.
</commit_message>
<xml_diff>
--- a/StoryCards.xlsx
+++ b/StoryCards.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="375" windowWidth="13875" windowHeight="5160"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="78">
   <si>
     <t>ID</t>
   </si>
@@ -241,13 +241,25 @@
   </si>
   <si>
     <t>6h</t>
+  </si>
+  <si>
+    <t>Recherche</t>
+  </si>
+  <si>
+    <t>Sammeln von infos zu Ameisensysteme</t>
+  </si>
+  <si>
+    <t>Sammeln von infos zu TSP</t>
+  </si>
+  <si>
+    <t>Komprimierung der gesammelten Daten</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,7 +360,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -422,6 +434,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -456,6 +469,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -631,14 +645,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -654,7 +668,7 @@
     <col min="13" max="13" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="33.75">
+    <row r="1" spans="1:14" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
         <v>18</v>
       </c>
@@ -663,7 +677,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -685,7 +699,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
@@ -701,7 +715,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -717,7 +731,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
@@ -730,7 +744,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="25.5">
+    <row r="7" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -772,7 +786,7 @@
       </c>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -813,7 +827,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -854,7 +868,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -895,7 +909,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -936,7 +950,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
@@ -977,7 +991,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
@@ -1018,7 +1032,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7</v>
       </c>
@@ -1050,7 +1064,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>8</v>
       </c>
@@ -1082,7 +1096,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>9</v>
       </c>
@@ -1120,7 +1134,7 @@
         <v>40847</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10</v>
       </c>
@@ -1152,7 +1166,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>11</v>
       </c>
@@ -1193,7 +1207,7 @@
         <v>40795</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>12</v>
       </c>
@@ -1234,7 +1248,7 @@
         <v>40822</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>13</v>
       </c>
@@ -1264,6 +1278,93 @@
       </c>
       <c r="K20" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="3">
+        <v>40823</v>
+      </c>
+      <c r="F21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" t="s">
+        <v>74</v>
+      </c>
+      <c r="I21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="3">
+        <v>40823</v>
+      </c>
+      <c r="F22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" t="s">
+        <v>74</v>
+      </c>
+      <c r="I22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>16</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="3">
+        <v>40823</v>
+      </c>
+      <c r="F23" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" t="s">
+        <v>58</v>
+      </c>
+      <c r="I23" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1316,24 +1417,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- updated StoryCards.xlsx - added Ordner Bilder für Präsi + 3 Bilder - added Infos zu Ameisensystemen & TSP.docx
</commit_message>
<xml_diff>
--- a/StoryCards.xlsx
+++ b/StoryCards.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="78">
   <si>
     <t>ID</t>
   </si>
@@ -649,7 +649,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1285,7 +1285,7 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
         <v>25</v>
@@ -1307,6 +1307,15 @@
       </c>
       <c r="I21" t="s">
         <v>75</v>
+      </c>
+      <c r="K21" t="s">
+        <v>54</v>
+      </c>
+      <c r="L21" t="s">
+        <v>52</v>
+      </c>
+      <c r="M21" s="3">
+        <v>40823</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1314,7 +1323,7 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
- added Bilder für Präsi/220px-TSP_Deutschland_3.png - updated Infos zu Ameisensystemen & TSP.docx - updated StoryCards.xlsx
</commit_message>
<xml_diff>
--- a/StoryCards.xlsx
+++ b/StoryCards.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="79">
   <si>
     <t>ID</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>Komprimierung der gesammelten Daten</t>
+  </si>
+  <si>
+    <t>1h 30min</t>
   </si>
 </sst>
 </file>
@@ -649,7 +652,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1323,7 +1326,7 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
         <v>25</v>
@@ -1348,6 +1351,12 @@
       </c>
       <c r="K22" t="s">
         <v>54</v>
+      </c>
+      <c r="L22" t="s">
+        <v>78</v>
+      </c>
+      <c r="M22" s="3">
+        <v>40823</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- beste Tour hervorgehoben - OP-Liste aktualisiert
</commit_message>
<xml_diff>
--- a/StoryCards.xlsx
+++ b/StoryCards.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="375" windowWidth="13875" windowHeight="5160"/>
+    <workbookView xWindow="837" yWindow="368" windowWidth="13881" windowHeight="5157"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$7:$M$34</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="80">
   <si>
     <t>ID</t>
   </si>
@@ -256,13 +256,16 @@
   </si>
   <si>
     <t>1h 30min</t>
+  </si>
+  <si>
+    <t>12h</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,7 +366,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -437,7 +440,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -472,7 +474,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -648,16 +649,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
@@ -671,7 +672,7 @@
     <col min="13" max="13" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="33.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:14" ht="33.5">
       <c r="A1" s="5" t="s">
         <v>18</v>
       </c>
@@ -680,7 +681,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -702,7 +703,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
@@ -718,7 +719,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -734,7 +735,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
@@ -747,7 +748,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="25.15">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -789,7 +790,7 @@
       </c>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="A8">
         <v>1</v>
       </c>
@@ -830,7 +831,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="A9">
         <v>2</v>
       </c>
@@ -871,7 +872,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="A10">
         <v>3</v>
       </c>
@@ -912,7 +913,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11">
         <v>4</v>
       </c>
@@ -953,7 +954,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="A12">
         <v>5</v>
       </c>
@@ -994,7 +995,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14">
       <c r="A13">
         <v>6</v>
       </c>
@@ -1035,7 +1036,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14">
       <c r="A14">
         <v>7</v>
       </c>
@@ -1066,8 +1067,14 @@
       <c r="K14" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>79</v>
+      </c>
+      <c r="M14" s="3">
+        <v>40823</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15">
         <v>8</v>
       </c>
@@ -1099,7 +1106,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14">
       <c r="A16">
         <v>9</v>
       </c>
@@ -1137,7 +1144,7 @@
         <v>40847</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13">
       <c r="A17">
         <v>10</v>
       </c>
@@ -1169,7 +1176,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13">
       <c r="A18">
         <v>11</v>
       </c>
@@ -1210,7 +1217,7 @@
         <v>40795</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13">
       <c r="A19">
         <v>12</v>
       </c>
@@ -1251,7 +1258,7 @@
         <v>40822</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13">
       <c r="A20">
         <v>13</v>
       </c>
@@ -1283,7 +1290,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13">
       <c r="A21">
         <v>14</v>
       </c>
@@ -1321,7 +1328,7 @@
         <v>40823</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13">
       <c r="A22">
         <v>15</v>
       </c>
@@ -1359,7 +1366,7 @@
         <v>40823</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13">
       <c r="A23">
         <v>16</v>
       </c>
@@ -1441,24 +1448,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- updated StoryCards.xlsx & TSP_Doku.docx 1. 2 neue StoryCards erstellt (Doku & Vortrag) 2. die beiden Rechnungen in den TSP Teil eingefügt
</commit_message>
<xml_diff>
--- a/StoryCards.xlsx
+++ b/StoryCards.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="837" yWindow="368" windowWidth="13881" windowHeight="5157"/>
+    <workbookView xWindow="840" yWindow="375" windowWidth="13875" windowHeight="5160"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="86">
   <si>
     <t>ID</t>
   </si>
@@ -259,13 +259,31 @@
   </si>
   <si>
     <t>12h</t>
+  </si>
+  <si>
+    <t>2h 30min</t>
+  </si>
+  <si>
+    <t>4h</t>
+  </si>
+  <si>
+    <t>Vortrag</t>
+  </si>
+  <si>
+    <t>Dokumentation</t>
+  </si>
+  <si>
+    <t>Präsentation erstellen</t>
+  </si>
+  <si>
+    <t>Dokumentation erstellen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -366,7 +384,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -440,6 +458,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -474,6 +493,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -649,14 +669,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C15" sqref="A15:XFD15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -666,13 +686,13 @@
     <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.28515625" customWidth="1"/>
     <col min="10" max="10" width="14.7109375" customWidth="1"/>
     <col min="11" max="12" width="14.5703125" customWidth="1"/>
     <col min="13" max="13" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="33.5">
+    <row r="1" spans="1:14" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
         <v>18</v>
       </c>
@@ -681,7 +701,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -703,7 +723,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
@@ -719,7 +739,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -735,7 +755,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
@@ -748,7 +768,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="25.15">
+    <row r="7" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -790,7 +810,7 @@
       </c>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -831,7 +851,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -872,7 +892,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -913,7 +933,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -954,7 +974,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
@@ -995,7 +1015,7 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
@@ -1036,12 +1056,12 @@
         <v>40794</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
         <v>24</v>
@@ -1064,6 +1084,9 @@
       <c r="I14" t="s">
         <v>56</v>
       </c>
+      <c r="J14" t="s">
+        <v>31</v>
+      </c>
       <c r="K14" t="s">
         <v>53</v>
       </c>
@@ -1074,7 +1097,7 @@
         <v>40823</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>8</v>
       </c>
@@ -1106,7 +1129,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>9</v>
       </c>
@@ -1144,7 +1167,7 @@
         <v>40847</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10</v>
       </c>
@@ -1176,7 +1199,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>11</v>
       </c>
@@ -1217,7 +1240,7 @@
         <v>40795</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>12</v>
       </c>
@@ -1258,12 +1281,12 @@
         <v>40822</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
         <v>24</v>
@@ -1286,11 +1309,14 @@
       <c r="I20" t="s">
         <v>67</v>
       </c>
+      <c r="J20" t="s">
+        <v>31</v>
+      </c>
       <c r="K20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>14</v>
       </c>
@@ -1318,6 +1344,9 @@
       <c r="I21" t="s">
         <v>75</v>
       </c>
+      <c r="J21" t="s">
+        <v>31</v>
+      </c>
       <c r="K21" t="s">
         <v>54</v>
       </c>
@@ -1328,7 +1357,7 @@
         <v>40823</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>15</v>
       </c>
@@ -1356,6 +1385,9 @@
       <c r="I22" t="s">
         <v>76</v>
       </c>
+      <c r="J22" t="s">
+        <v>31</v>
+      </c>
       <c r="K22" t="s">
         <v>54</v>
       </c>
@@ -1366,12 +1398,12 @@
         <v>40823</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
         <v>24</v>
@@ -1394,8 +1426,81 @@
       <c r="I23" t="s">
         <v>77</v>
       </c>
+      <c r="J23" t="s">
+        <v>31</v>
+      </c>
       <c r="K23" t="s">
         <v>52</v>
+      </c>
+      <c r="L23" t="s">
+        <v>80</v>
+      </c>
+      <c r="M23" s="3">
+        <v>40830</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>17</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" s="3">
+        <v>40840</v>
+      </c>
+      <c r="F24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" t="s">
+        <v>71</v>
+      </c>
+      <c r="H24" t="s">
+        <v>58</v>
+      </c>
+      <c r="I24" t="s">
+        <v>84</v>
+      </c>
+      <c r="K24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>18</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="3">
+        <v>40840</v>
+      </c>
+      <c r="F25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" t="s">
+        <v>71</v>
+      </c>
+      <c r="H25" t="s">
+        <v>58</v>
+      </c>
+      <c r="I25" t="s">
+        <v>85</v>
+      </c>
+      <c r="K25" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1448,24 +1553,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>